<commit_message>
NUWA MAM CONTINUW AND vALUATED PASHIKHEL
</commit_message>
<xml_diff>
--- a/ofc/estimates/pashikhel park/V pasikhel park.xlsx
+++ b/ofc/estimates/pashikhel park/V pasikhel park.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="finalized" sheetId="19" r:id="rId1"/>
@@ -47,7 +47,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="2">Estimate!$A$1:$K$71</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'Estimate (2)'!$A$1:$K$90</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">finalized!$A$1:$K$89</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">V!$A$1:$K$89</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">V!$A$1:$K$57</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">Estimate!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="3">'Estimate (2)'!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">finalized!$1:$8</definedName>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="83">
   <si>
     <t>Government of Nepal</t>
   </si>
@@ -654,22 +654,35 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -677,9 +690,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -696,30 +706,20 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1339,7 +1339,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S146"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A7" sqref="A7:F7"/>
     </sheetView>
   </sheetViews>
@@ -1358,116 +1358,116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-      <c r="I1" s="85"/>
-      <c r="J1" s="85"/>
-      <c r="K1" s="85"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
     </row>
     <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="74"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="74"/>
-      <c r="J3" s="74"/>
-      <c r="K3" s="74"/>
+      <c r="B3" s="79"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="79"/>
     </row>
     <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="74" t="s">
+      <c r="A4" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="74"/>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="74"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="74"/>
-      <c r="J4" s="74"/>
-      <c r="K4" s="74"/>
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="79"/>
     </row>
     <row r="5" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="87" t="s">
+      <c r="A5" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="87"/>
-      <c r="C5" s="87"/>
-      <c r="D5" s="87"/>
-      <c r="E5" s="87"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="87"/>
-      <c r="H5" s="87"/>
-      <c r="I5" s="87"/>
-      <c r="J5" s="87"/>
-      <c r="K5" s="87"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
+      <c r="I5" s="80"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="80"/>
     </row>
     <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="78" t="s">
+      <c r="A6" s="75" t="s">
         <v>78</v>
       </c>
-      <c r="B6" s="78"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="84" t="s">
+      <c r="H6" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="84"/>
-      <c r="J6" s="84"/>
-      <c r="K6" s="84"/>
+      <c r="I6" s="76"/>
+      <c r="J6" s="76"/>
+      <c r="K6" s="76"/>
       <c r="O6" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="89" t="s">
+      <c r="A7" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="89"/>
-      <c r="C7" s="89"/>
-      <c r="D7" s="89"/>
-      <c r="E7" s="89"/>
-      <c r="F7" s="89"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="72"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="90" t="s">
+      <c r="H7" s="73" t="s">
         <v>77</v>
       </c>
-      <c r="I7" s="90"/>
-      <c r="J7" s="90"/>
-      <c r="K7" s="90"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="73"/>
     </row>
     <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -3381,11 +3381,11 @@
       <c r="B84" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C84" s="88">
+      <c r="C84" s="71">
         <f>J82</f>
         <v>658753.39262024697</v>
       </c>
-      <c r="D84" s="88"/>
+      <c r="D84" s="71"/>
       <c r="E84" s="39">
         <v>100</v>
       </c>
@@ -3401,11 +3401,11 @@
       <c r="B85" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C85" s="91">
+      <c r="C85" s="74">
         <f>500000+86000</f>
         <v>586000</v>
       </c>
-      <c r="D85" s="91"/>
+      <c r="D85" s="74"/>
       <c r="E85" s="39"/>
       <c r="F85" s="49"/>
       <c r="G85" s="48"/>
@@ -3419,11 +3419,11 @@
       <c r="B86" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C86" s="91">
+      <c r="C86" s="74">
         <f>C85-C88-C89</f>
         <v>556700</v>
       </c>
-      <c r="D86" s="91"/>
+      <c r="D86" s="74"/>
       <c r="E86" s="39">
         <f>C86/C84*100</f>
         <v>84.508103675288709</v>
@@ -3440,11 +3440,11 @@
       <c r="B87" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C87" s="88">
+      <c r="C87" s="71">
         <f>C84-C86</f>
         <v>102053.39262024697</v>
       </c>
-      <c r="D87" s="88"/>
+      <c r="D87" s="71"/>
       <c r="E87" s="39">
         <f>100-E86</f>
         <v>15.491896324711291</v>
@@ -3461,11 +3461,11 @@
       <c r="B88" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C88" s="88">
+      <c r="C88" s="71">
         <f>C85*0.03</f>
         <v>17580</v>
       </c>
-      <c r="D88" s="88"/>
+      <c r="D88" s="71"/>
       <c r="E88" s="39">
         <v>3</v>
       </c>
@@ -3481,11 +3481,11 @@
       <c r="B89" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C89" s="88">
+      <c r="C89" s="71">
         <f>C85*0.02</f>
         <v>11720</v>
       </c>
-      <c r="D89" s="88"/>
+      <c r="D89" s="71"/>
       <c r="E89" s="39">
         <v>2</v>
       </c>
@@ -3567,6 +3567,13 @@
     <row r="146" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C88:D88"/>
     <mergeCell ref="C89:D89"/>
     <mergeCell ref="A7:F7"/>
@@ -3575,13 +3582,6 @@
     <mergeCell ref="C85:D85"/>
     <mergeCell ref="C86:D86"/>
     <mergeCell ref="C87:D87"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
@@ -3595,7 +3595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -3615,90 +3615,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="90" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="90"/>
+      <c r="K1" s="90"/>
     </row>
     <row r="2" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
+      <c r="B2" s="91"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="74"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="74"/>
-      <c r="J3" s="74"/>
-      <c r="K3" s="74"/>
+      <c r="B3" s="79"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="79"/>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="74" t="s">
+      <c r="A4" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="74"/>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="74"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="74"/>
-      <c r="J4" s="74"/>
-      <c r="K4" s="74"/>
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="79"/>
     </row>
     <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="75" t="s">
+      <c r="A5" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="75"/>
-      <c r="C5" s="75"/>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="75"/>
-      <c r="H5" s="75"/>
-      <c r="I5" s="75"/>
-      <c r="J5" s="75"/>
-      <c r="K5" s="75"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
+      <c r="F5" s="92"/>
+      <c r="G5" s="92"/>
+      <c r="H5" s="92"/>
+      <c r="I5" s="92"/>
+      <c r="J5" s="92"/>
+      <c r="K5" s="92"/>
     </row>
     <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="70">
+      <c r="C6" s="88">
         <f>F36</f>
         <v>658753.39262024697</v>
       </c>
-      <c r="D6" s="71"/>
+      <c r="D6" s="89"/>
       <c r="E6" s="9"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -3706,11 +3706,11 @@
         <v>20</v>
       </c>
       <c r="I6" s="8"/>
-      <c r="J6" s="70">
+      <c r="J6" s="88">
         <f>I36</f>
-        <v>614393.61235914705</v>
-      </c>
-      <c r="K6" s="71"/>
+        <v>614864.14527368033</v>
+      </c>
+      <c r="K6" s="89"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
@@ -3719,77 +3719,77 @@
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="F7" s="79"/>
-      <c r="G7" s="79"/>
-      <c r="I7" s="80" t="s">
+      <c r="F7" s="83"/>
+      <c r="G7" s="83"/>
+      <c r="I7" s="84" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="80"/>
-      <c r="K7" s="80"/>
+      <c r="J7" s="84"/>
+      <c r="K7" s="84"/>
     </row>
     <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="78" t="str">
+      <c r="A8" s="75" t="str">
         <f>finalized!A6</f>
         <v xml:space="preserve">Project:- पासीखेलमा भएको पाटी संरक्षण </v>
       </c>
-      <c r="B8" s="78"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="78"/>
-      <c r="F8" s="78"/>
-      <c r="I8" s="81" t="s">
+      <c r="B8" s="75"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="75"/>
+      <c r="I8" s="85" t="s">
         <v>81</v>
       </c>
-      <c r="J8" s="81"/>
-      <c r="K8" s="81"/>
+      <c r="J8" s="85"/>
+      <c r="K8" s="85"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="82" t="str">
+      <c r="A9" s="86" t="str">
         <f>finalized!A7</f>
         <v>Location:- Shankharapur Municipality 9</v>
       </c>
-      <c r="B9" s="82"/>
-      <c r="C9" s="82"/>
-      <c r="D9" s="82"/>
-      <c r="E9" s="82"/>
-      <c r="F9" s="82"/>
-      <c r="I9" s="81" t="s">
+      <c r="B9" s="86"/>
+      <c r="C9" s="86"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="86"/>
+      <c r="F9" s="86"/>
+      <c r="I9" s="85" t="s">
         <v>82</v>
       </c>
-      <c r="J9" s="81"/>
-      <c r="K9" s="81"/>
+      <c r="J9" s="85"/>
+      <c r="K9" s="85"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="76" t="s">
+      <c r="A11" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="76" t="s">
+      <c r="B11" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="76" t="s">
+      <c r="C11" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="83" t="s">
+      <c r="D11" s="87" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="83"/>
-      <c r="F11" s="83"/>
-      <c r="G11" s="83" t="s">
+      <c r="E11" s="87"/>
+      <c r="F11" s="87"/>
+      <c r="G11" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="83"/>
-      <c r="I11" s="83"/>
-      <c r="J11" s="76" t="s">
+      <c r="H11" s="87"/>
+      <c r="I11" s="87"/>
+      <c r="J11" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="77" t="s">
+      <c r="K11" s="82" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="76"/>
-      <c r="B12" s="76"/>
-      <c r="C12" s="76"/>
+      <c r="A12" s="81"/>
+      <c r="B12" s="81"/>
+      <c r="C12" s="81"/>
       <c r="D12" s="11" t="s">
         <v>26</v>
       </c>
@@ -3808,8 +3808,8 @@
       <c r="I12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="76"/>
-      <c r="K12" s="77"/>
+      <c r="J12" s="81"/>
+      <c r="K12" s="82"/>
     </row>
     <row r="13" spans="1:11" s="1" customFormat="1" ht="149.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="27">
@@ -3837,26 +3837,26 @@
         <v>2889.2195199999992</v>
       </c>
       <c r="G13" s="12">
-        <f>V!G14</f>
-        <v>26.68</v>
+        <f>V!G12</f>
+        <v>26.846250000000005</v>
       </c>
       <c r="H13" s="12">
-        <f>V!I14</f>
+        <f>V!I12</f>
         <v>64.63</v>
       </c>
       <c r="I13" s="12">
         <f>G13*H13</f>
-        <v>1724.3283999999999</v>
+        <v>1735.0731375000003</v>
       </c>
       <c r="J13" s="28">
         <f>I13-F13</f>
-        <v>-1164.8911199999993</v>
+        <v>-1154.1463824999989</v>
       </c>
       <c r="K13" s="14"/>
     </row>
     <row r="14" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="27"/>
-      <c r="B14" s="92" t="str">
+      <c r="B14" s="70" t="str">
         <f>finalized!B15</f>
         <v>VAT calculation</v>
       </c>
@@ -3870,8 +3870,8 @@
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
       <c r="I14" s="12">
-        <f>V!J15</f>
-        <v>185.79062666666667</v>
+        <f>V!J13</f>
+        <v>186.94833625000004</v>
       </c>
       <c r="J14" s="28"/>
       <c r="K14" s="14"/>
@@ -3915,26 +3915,26 @@
         <v>23003.795789999996</v>
       </c>
       <c r="G16" s="12">
-        <f>V!G26</f>
-        <v>4.9664999999999999</v>
+        <f>V!G19</f>
+        <v>4.2914999999999992</v>
       </c>
       <c r="H16" s="12">
-        <f>V!I26</f>
+        <f>V!I19</f>
         <v>4561.53</v>
       </c>
       <c r="I16" s="12">
         <f>G16*H16</f>
-        <v>22654.838744999997</v>
+        <v>19575.805994999995</v>
       </c>
       <c r="J16" s="28">
         <f>I16-F16</f>
-        <v>-348.9570449999992</v>
+        <v>-3427.9897950000013</v>
       </c>
       <c r="K16" s="14"/>
     </row>
     <row r="17" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="27"/>
-      <c r="B17" s="92" t="str">
+      <c r="B17" s="70" t="str">
         <f>finalized!B35</f>
         <v>VAT calculation</v>
       </c>
@@ -3948,8 +3948,8 @@
       <c r="G17" s="12"/>
       <c r="H17" s="12"/>
       <c r="I17" s="12">
-        <f>V!J27</f>
-        <v>1995.3787854</v>
+        <f>V!J20</f>
+        <v>1724.1856553999996</v>
       </c>
       <c r="J17" s="28"/>
       <c r="K17" s="14"/>
@@ -3993,11 +3993,11 @@
         <v>22055.952999999998</v>
       </c>
       <c r="G19" s="12">
-        <f>V!G34</f>
+        <f>V!G25</f>
         <v>2.0282499999999999</v>
       </c>
       <c r="H19" s="12">
-        <f>V!I34</f>
+        <f>V!I25</f>
         <v>10634.5</v>
       </c>
       <c r="I19" s="12">
@@ -4012,7 +4012,7 @@
     </row>
     <row r="20" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="27"/>
-      <c r="B20" s="92" t="str">
+      <c r="B20" s="70" t="str">
         <f>finalized!B35</f>
         <v>VAT calculation</v>
       </c>
@@ -4026,7 +4026,7 @@
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
       <c r="I20" s="12">
-        <f>V!J35</f>
+        <f>V!J26</f>
         <v>2127.7069965666665</v>
       </c>
       <c r="J20" s="28"/>
@@ -4071,26 +4071,26 @@
         <v>493860.44752000005</v>
       </c>
       <c r="G22" s="12">
-        <f>V!G39</f>
-        <v>46.81600000000001</v>
+        <f>V!G30</f>
+        <v>47.181750000000008</v>
       </c>
       <c r="H22" s="12">
-        <f>V!I39</f>
+        <f>V!I30</f>
         <v>9709.43</v>
       </c>
       <c r="I22" s="12">
         <f>G22*H22</f>
-        <v>454556.67488000012</v>
+        <v>458107.89890250011</v>
       </c>
       <c r="J22" s="28">
         <f>I22-F22</f>
-        <v>-39303.772639999923</v>
+        <v>-35752.548617499939</v>
       </c>
       <c r="K22" s="14"/>
     </row>
     <row r="23" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="27"/>
-      <c r="B23" s="92" t="str">
+      <c r="B23" s="70" t="str">
         <f>finalized!B40</f>
         <v>VAT calculation</v>
       </c>
@@ -4104,8 +4104,8 @@
       <c r="G23" s="12"/>
       <c r="H23" s="12"/>
       <c r="I23" s="12">
-        <f>V!J40</f>
-        <v>32976.937593600007</v>
+        <f>V!J31</f>
+        <v>33234.569918550005</v>
       </c>
       <c r="J23" s="28"/>
       <c r="K23" s="14"/>
@@ -4149,11 +4149,11 @@
         <v>6452.2148148148144</v>
       </c>
       <c r="G25" s="12">
-        <f>V!G45</f>
+        <f>V!G36</f>
         <v>5.1975308641975304E-2</v>
       </c>
       <c r="H25" s="12">
-        <f>V!I45</f>
+        <f>V!I36</f>
         <v>124140</v>
       </c>
       <c r="I25" s="12">
@@ -4168,7 +4168,7 @@
     </row>
     <row r="26" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="27"/>
-      <c r="B26" s="92" t="str">
+      <c r="B26" s="70" t="str">
         <f>finalized!B46</f>
         <v>VAT calculation</v>
       </c>
@@ -4182,7 +4182,7 @@
       <c r="G26" s="12"/>
       <c r="H26" s="12"/>
       <c r="I26" s="12">
-        <f>V!J46</f>
+        <f>V!J37</f>
         <v>749.73343209876532</v>
       </c>
       <c r="J26" s="28"/>
@@ -4227,11 +4227,11 @@
         <v>10429.352999999999</v>
       </c>
       <c r="G28" s="12">
-        <f>V!G50</f>
+        <f>V!G41</f>
         <v>0.89999999999999991</v>
       </c>
       <c r="H28" s="12">
-        <f>V!I50</f>
+        <f>V!I41</f>
         <v>11588.17</v>
       </c>
       <c r="I28" s="12">
@@ -4246,7 +4246,7 @@
     </row>
     <row r="29" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="27"/>
-      <c r="B29" s="92" t="str">
+      <c r="B29" s="70" t="str">
         <f>finalized!B51</f>
         <v>VAT calculation</v>
       </c>
@@ -4260,7 +4260,7 @@
       <c r="G29" s="12"/>
       <c r="H29" s="12"/>
       <c r="I29" s="12">
-        <f>V!J51</f>
+        <f>V!J42</f>
         <v>1055.7120600000001</v>
       </c>
       <c r="J29" s="28"/>
@@ -4305,11 +4305,11 @@
         <v>51449.599999999999</v>
       </c>
       <c r="G31" s="12">
-        <f>V!G54</f>
+        <f>V!G45</f>
         <v>10</v>
       </c>
       <c r="H31" s="12">
-        <f>V!I54</f>
+        <f>V!I45</f>
         <v>5144.96</v>
       </c>
       <c r="I31" s="12">
@@ -4324,7 +4324,7 @@
     </row>
     <row r="32" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="27"/>
-      <c r="B32" s="92" t="str">
+      <c r="B32" s="70" t="str">
         <f>finalized!B55</f>
         <v>VAT calculation</v>
       </c>
@@ -4338,7 +4338,7 @@
       <c r="G32" s="12"/>
       <c r="H32" s="12"/>
       <c r="I32" s="12">
-        <f>V!J55</f>
+        <f>V!J46</f>
         <v>5965.9183999999996</v>
       </c>
       <c r="J32" s="28"/>
@@ -4383,11 +4383,11 @@
         <v>500</v>
       </c>
       <c r="G34" s="12">
-        <f>V!G80</f>
+        <f>V!G48</f>
         <v>1</v>
       </c>
       <c r="H34" s="12">
-        <f>V!I80</f>
+        <f>V!I48</f>
         <v>500</v>
       </c>
       <c r="I34" s="12">
@@ -4429,16 +4429,23 @@
       <c r="H36" s="7"/>
       <c r="I36" s="7">
         <f>SUM(I13:I34)</f>
-        <v>614393.61235914705</v>
+        <v>614864.14527368033</v>
       </c>
       <c r="J36" s="13">
         <f>I36-F36</f>
-        <v>-44359.780261099921</v>
+        <v>-43889.247346566641</v>
       </c>
       <c r="K36" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -4452,13 +4459,6 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -4495,116 +4495,116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-      <c r="I1" s="85"/>
-      <c r="J1" s="85"/>
-      <c r="K1" s="85"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
     </row>
     <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="74"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="74"/>
-      <c r="J3" s="74"/>
-      <c r="K3" s="74"/>
+      <c r="B3" s="79"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="79"/>
     </row>
     <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="74" t="s">
+      <c r="A4" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="74"/>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="74"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="74"/>
-      <c r="J4" s="74"/>
-      <c r="K4" s="74"/>
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="79"/>
     </row>
     <row r="5" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="87" t="s">
+      <c r="A5" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="87"/>
-      <c r="C5" s="87"/>
-      <c r="D5" s="87"/>
-      <c r="E5" s="87"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="87"/>
-      <c r="H5" s="87"/>
-      <c r="I5" s="87"/>
-      <c r="J5" s="87"/>
-      <c r="K5" s="87"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
+      <c r="I5" s="80"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="80"/>
     </row>
     <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="78" t="s">
+      <c r="A6" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="78"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="84" t="s">
+      <c r="H6" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="84"/>
-      <c r="J6" s="84"/>
-      <c r="K6" s="84"/>
+      <c r="I6" s="76"/>
+      <c r="J6" s="76"/>
+      <c r="K6" s="76"/>
       <c r="O6" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="89" t="s">
+      <c r="A7" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="89"/>
-      <c r="C7" s="89"/>
-      <c r="D7" s="89"/>
-      <c r="E7" s="89"/>
-      <c r="F7" s="89"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="72"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="90" t="s">
+      <c r="H7" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="I7" s="90"/>
-      <c r="J7" s="90"/>
-      <c r="K7" s="90"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="73"/>
     </row>
     <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -6080,11 +6080,11 @@
       <c r="B66" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C66" s="88">
+      <c r="C66" s="71">
         <f>J64</f>
         <v>562056.0280514101</v>
       </c>
-      <c r="D66" s="88"/>
+      <c r="D66" s="71"/>
       <c r="E66" s="39">
         <v>100</v>
       </c>
@@ -6100,10 +6100,10 @@
       <c r="B67" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C67" s="91">
+      <c r="C67" s="74">
         <v>500000</v>
       </c>
-      <c r="D67" s="91"/>
+      <c r="D67" s="74"/>
       <c r="E67" s="39"/>
       <c r="F67" s="49"/>
       <c r="G67" s="48"/>
@@ -6117,11 +6117,11 @@
       <c r="B68" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C68" s="91">
+      <c r="C68" s="74">
         <f>C67-C70-C71</f>
         <v>475000</v>
       </c>
-      <c r="D68" s="91"/>
+      <c r="D68" s="74"/>
       <c r="E68" s="39">
         <f>C68/C66*100</f>
         <v>84.511147695857957</v>
@@ -6138,11 +6138,11 @@
       <c r="B69" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C69" s="88">
+      <c r="C69" s="71">
         <f>C66-C68</f>
         <v>87056.028051410103</v>
       </c>
-      <c r="D69" s="88"/>
+      <c r="D69" s="71"/>
       <c r="E69" s="39">
         <f>100-E68</f>
         <v>15.488852304142043</v>
@@ -6159,11 +6159,11 @@
       <c r="B70" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C70" s="88">
+      <c r="C70" s="71">
         <f>C67*0.03</f>
         <v>15000</v>
       </c>
-      <c r="D70" s="88"/>
+      <c r="D70" s="71"/>
       <c r="E70" s="39">
         <v>3</v>
       </c>
@@ -6179,11 +6179,11 @@
       <c r="B71" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C71" s="88">
+      <c r="C71" s="71">
         <f>C67*0.02</f>
         <v>10000</v>
       </c>
-      <c r="D71" s="88"/>
+      <c r="D71" s="71"/>
       <c r="E71" s="39">
         <v>2</v>
       </c>
@@ -6265,6 +6265,13 @@
     <row r="128" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C70:D70"/>
     <mergeCell ref="C71:D71"/>
     <mergeCell ref="A7:F7"/>
@@ -6273,13 +6280,6 @@
     <mergeCell ref="C67:D67"/>
     <mergeCell ref="C68:D68"/>
     <mergeCell ref="C69:D69"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
@@ -6315,116 +6315,116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-      <c r="I1" s="85"/>
-      <c r="J1" s="85"/>
-      <c r="K1" s="85"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
     </row>
     <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="74"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="74"/>
-      <c r="J3" s="74"/>
-      <c r="K3" s="74"/>
+      <c r="B3" s="79"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="79"/>
     </row>
     <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="74" t="s">
+      <c r="A4" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="74"/>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="74"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="74"/>
-      <c r="J4" s="74"/>
-      <c r="K4" s="74"/>
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="79"/>
     </row>
     <row r="5" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="87" t="s">
+      <c r="A5" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="87"/>
-      <c r="C5" s="87"/>
-      <c r="D5" s="87"/>
-      <c r="E5" s="87"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="87"/>
-      <c r="H5" s="87"/>
-      <c r="I5" s="87"/>
-      <c r="J5" s="87"/>
-      <c r="K5" s="87"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
+      <c r="I5" s="80"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="80"/>
     </row>
     <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="78" t="s">
+      <c r="A6" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="78"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="84" t="s">
+      <c r="H6" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="84"/>
-      <c r="J6" s="84"/>
-      <c r="K6" s="84"/>
+      <c r="I6" s="76"/>
+      <c r="J6" s="76"/>
+      <c r="K6" s="76"/>
       <c r="O6" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="89" t="s">
+      <c r="A7" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="89"/>
-      <c r="C7" s="89"/>
-      <c r="D7" s="89"/>
-      <c r="E7" s="89"/>
-      <c r="F7" s="89"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="72"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="90" t="s">
+      <c r="H7" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="I7" s="90"/>
-      <c r="J7" s="90"/>
-      <c r="K7" s="90"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="73"/>
     </row>
     <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -8369,11 +8369,11 @@
       <c r="B85" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C85" s="88">
+      <c r="C85" s="71">
         <f>J83</f>
         <v>655191.81745519862</v>
       </c>
-      <c r="D85" s="88"/>
+      <c r="D85" s="71"/>
       <c r="E85" s="39">
         <v>100</v>
       </c>
@@ -8389,11 +8389,11 @@
       <c r="B86" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C86" s="91">
+      <c r="C86" s="74">
         <f>500000+86000</f>
         <v>586000</v>
       </c>
-      <c r="D86" s="91"/>
+      <c r="D86" s="74"/>
       <c r="E86" s="39"/>
       <c r="F86" s="49"/>
       <c r="G86" s="48"/>
@@ -8407,11 +8407,11 @@
       <c r="B87" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C87" s="91">
+      <c r="C87" s="74">
         <f>C86-C89-C90</f>
         <v>556700</v>
       </c>
-      <c r="D87" s="91"/>
+      <c r="D87" s="74"/>
       <c r="E87" s="39">
         <f>C87/C85*100</f>
         <v>84.967483593164161</v>
@@ -8428,11 +8428,11 @@
       <c r="B88" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C88" s="88">
+      <c r="C88" s="71">
         <f>C85-C87</f>
         <v>98491.817455198616</v>
       </c>
-      <c r="D88" s="88"/>
+      <c r="D88" s="71"/>
       <c r="E88" s="39">
         <f>100-E87</f>
         <v>15.032516406835839</v>
@@ -8449,11 +8449,11 @@
       <c r="B89" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C89" s="88">
+      <c r="C89" s="71">
         <f>C86*0.03</f>
         <v>17580</v>
       </c>
-      <c r="D89" s="88"/>
+      <c r="D89" s="71"/>
       <c r="E89" s="39">
         <v>3</v>
       </c>
@@ -8469,11 +8469,11 @@
       <c r="B90" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C90" s="88">
+      <c r="C90" s="71">
         <f>C86*0.02</f>
         <v>11720</v>
       </c>
-      <c r="D90" s="88"/>
+      <c r="D90" s="71"/>
       <c r="E90" s="39">
         <v>2</v>
       </c>
@@ -8555,6 +8555,13 @@
     <row r="147" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C89:D89"/>
     <mergeCell ref="C90:D90"/>
     <mergeCell ref="A7:F7"/>
@@ -8563,13 +8570,6 @@
     <mergeCell ref="C86:D86"/>
     <mergeCell ref="C87:D87"/>
     <mergeCell ref="C88:D88"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
@@ -8584,10 +8584,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S146"/>
+  <dimension ref="A1:S114"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8605,116 +8605,116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-      <c r="I1" s="85"/>
-      <c r="J1" s="85"/>
-      <c r="K1" s="85"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
     </row>
     <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="74"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="74"/>
-      <c r="J3" s="74"/>
-      <c r="K3" s="74"/>
+      <c r="B3" s="79"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="79"/>
     </row>
     <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="74" t="s">
+      <c r="A4" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="74"/>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="74"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="74"/>
-      <c r="J4" s="74"/>
-      <c r="K4" s="74"/>
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="79"/>
     </row>
     <row r="5" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="87" t="s">
+      <c r="A5" s="80" t="s">
         <v>79</v>
       </c>
-      <c r="B5" s="87"/>
-      <c r="C5" s="87"/>
-      <c r="D5" s="87"/>
-      <c r="E5" s="87"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="87"/>
-      <c r="H5" s="87"/>
-      <c r="I5" s="87"/>
-      <c r="J5" s="87"/>
-      <c r="K5" s="87"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
+      <c r="I5" s="80"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="80"/>
     </row>
     <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="78" t="s">
+      <c r="A6" s="75" t="s">
         <v>78</v>
       </c>
-      <c r="B6" s="78"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="84" t="s">
+      <c r="H6" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="84"/>
-      <c r="J6" s="84"/>
-      <c r="K6" s="84"/>
+      <c r="I6" s="76"/>
+      <c r="J6" s="76"/>
+      <c r="K6" s="76"/>
       <c r="O6" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="89" t="s">
+      <c r="A7" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="89"/>
-      <c r="C7" s="89"/>
-      <c r="D7" s="89"/>
-      <c r="E7" s="89"/>
-      <c r="F7" s="89"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="72"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="90" t="s">
+      <c r="H7" s="73" t="s">
         <v>77</v>
       </c>
-      <c r="I7" s="90"/>
-      <c r="J7" s="90"/>
-      <c r="K7" s="90"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="73"/>
     </row>
     <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -8786,19 +8786,19 @@
         <v>0.5</v>
       </c>
       <c r="D10" s="38">
-        <f>D38</f>
+        <f>D29</f>
         <v>13.3</v>
       </c>
       <c r="E10" s="38">
-        <f>F38/2</f>
-        <v>1.6</v>
+        <f>F29/2</f>
+        <v>1.6125</v>
       </c>
       <c r="F10" s="38">
         <v>2</v>
       </c>
       <c r="G10" s="39">
         <f>PRODUCT(C10:F10)</f>
-        <v>21.28</v>
+        <v>21.446250000000003</v>
       </c>
       <c r="H10" s="40"/>
       <c r="I10" s="40"/>
@@ -8845,31 +8845,29 @@
       <c r="R11" s="25"/>
       <c r="S11" s="25"/>
     </row>
-    <row r="12" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18"/>
       <c r="B12" s="37" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="36">
-        <v>0</v>
-      </c>
-      <c r="D12" s="38">
-        <f>21.93+3.04</f>
-        <v>24.97</v>
-      </c>
-      <c r="E12" s="38">
-        <v>2.9</v>
-      </c>
-      <c r="F12" s="38">
-        <v>0.15</v>
-      </c>
-      <c r="G12" s="39">
-        <f>PRODUCT(C12:F12)</f>
-        <v>0</v>
-      </c>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
-      <c r="J12" s="40"/>
+        <v>40</v>
+      </c>
+      <c r="C12" s="19"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="23">
+        <f>SUM(G10:G11)</f>
+        <v>26.846250000000005</v>
+      </c>
+      <c r="H12" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12" s="23">
+        <v>64.63</v>
+      </c>
+      <c r="J12" s="41">
+        <f>G12*I12</f>
+        <v>1735.0731375000003</v>
+      </c>
       <c r="K12" s="21"/>
       <c r="M12" s="25"/>
       <c r="N12" s="1"/>
@@ -8879,31 +8877,22 @@
       <c r="R12" s="25"/>
       <c r="S12" s="25"/>
     </row>
-    <row r="13" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
       <c r="B13" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="36">
-        <v>0</v>
-      </c>
-      <c r="D13" s="38">
-        <f>(11.17*2+4.42+12.25)/3.281</f>
-        <v>11.889667784212129</v>
-      </c>
-      <c r="E13" s="38">
-        <v>1.3</v>
-      </c>
-      <c r="F13" s="38">
-        <v>0.15</v>
-      </c>
-      <c r="G13" s="39">
-        <f>PRODUCT(C13:F13)</f>
-        <v>0</v>
-      </c>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
-      <c r="J13" s="40"/>
+        <v>38</v>
+      </c>
+      <c r="C13" s="19"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="41">
+        <f>0.13*G12*19284/360</f>
+        <v>186.94833625000004</v>
+      </c>
       <c r="K13" s="21"/>
       <c r="M13" s="25"/>
       <c r="N13" s="1"/>
@@ -8915,27 +8904,15 @@
     </row>
     <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18"/>
-      <c r="B14" s="37" t="s">
-        <v>40</v>
-      </c>
+      <c r="B14" s="37"/>
       <c r="C14" s="19"/>
       <c r="D14" s="20"/>
       <c r="E14" s="21"/>
       <c r="F14" s="21"/>
-      <c r="G14" s="23">
-        <f>SUM(G10:G11)</f>
-        <v>26.68</v>
-      </c>
-      <c r="H14" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="I14" s="23">
-        <v>64.63</v>
-      </c>
-      <c r="J14" s="41">
-        <f>G14*I14</f>
-        <v>1724.3283999999999</v>
-      </c>
+      <c r="G14" s="23"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="41"/>
       <c r="K14" s="21"/>
       <c r="M14" s="25"/>
       <c r="N14" s="1"/>
@@ -8945,10 +8922,12 @@
       <c r="R14" s="25"/>
       <c r="S14" s="25"/>
     </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="18"/>
-      <c r="B15" s="37" t="s">
-        <v>38</v>
+    <row r="15" spans="1:19" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="18">
+        <v>2</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>43</v>
       </c>
       <c r="C15" s="19"/>
       <c r="D15" s="20"/>
@@ -8957,10 +8936,7 @@
       <c r="G15" s="23"/>
       <c r="H15" s="22"/>
       <c r="I15" s="23"/>
-      <c r="J15" s="41">
-        <f>0.13*G14*19284/360</f>
-        <v>185.79062666666667</v>
-      </c>
+      <c r="J15" s="41"/>
       <c r="K15" s="21"/>
       <c r="M15" s="25"/>
       <c r="N15" s="1"/>
@@ -8972,15 +8948,30 @@
     </row>
     <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="41"/>
+      <c r="B16" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="36">
+        <v>1</v>
+      </c>
+      <c r="D16" s="38">
+        <f>D23</f>
+        <v>13.3</v>
+      </c>
+      <c r="E16" s="38">
+        <f>E23</f>
+        <v>1.7</v>
+      </c>
+      <c r="F16" s="38">
+        <v>0.15</v>
+      </c>
+      <c r="G16" s="39">
+        <f>PRODUCT(C16:F16)</f>
+        <v>3.3914999999999997</v>
+      </c>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
       <c r="K16" s="21"/>
       <c r="M16" s="25"/>
       <c r="N16" s="1"/>
@@ -8990,21 +8981,30 @@
       <c r="R16" s="25"/>
       <c r="S16" s="25"/>
     </row>
-    <row r="17" spans="1:19" ht="96.6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="18">
-        <v>2</v>
-      </c>
-      <c r="B17" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="41"/>
+    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="18"/>
+      <c r="B17" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="36">
+        <v>0</v>
+      </c>
+      <c r="D17" s="38">
+        <v>10</v>
+      </c>
+      <c r="E17" s="38">
+        <v>0.45</v>
+      </c>
+      <c r="F17" s="38">
+        <v>0.15</v>
+      </c>
+      <c r="G17" s="39">
+        <f t="shared" ref="G17:G18" si="1">PRODUCT(C17:F17)</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
       <c r="K17" s="21"/>
       <c r="M17" s="25"/>
       <c r="N17" s="1"/>
@@ -9014,27 +9014,24 @@
       <c r="R17" s="25"/>
       <c r="S17" s="25"/>
     </row>
-    <row r="18" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="18"/>
-      <c r="B18" s="37" t="s">
-        <v>41</v>
-      </c>
+      <c r="B18" s="37"/>
       <c r="C18" s="36">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D18" s="38">
-        <f>D22</f>
-        <v>13.3</v>
+        <v>10</v>
       </c>
       <c r="E18" s="38">
         <v>0.6</v>
       </c>
       <c r="F18" s="38">
-        <v>1</v>
+        <v>0.15</v>
       </c>
       <c r="G18" s="39">
-        <f>0*PRODUCT(C18:F18)</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.89999999999999991</v>
       </c>
       <c r="H18" s="40"/>
       <c r="I18" s="40"/>
@@ -9048,108 +9045,77 @@
       <c r="R18" s="25"/>
       <c r="S18" s="25"/>
     </row>
-    <row r="19" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="18"/>
+    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="40"/>
       <c r="B19" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="23">
-        <f>SUM(G18:G18)</f>
-        <v>0</v>
-      </c>
-      <c r="H19" s="22" t="s">
+      <c r="C19" s="42"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="33">
+        <f>SUM(G16:G18)</f>
+        <v>4.2914999999999992</v>
+      </c>
+      <c r="H19" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="I19" s="23">
-        <v>404.28</v>
-      </c>
-      <c r="J19" s="41">
+      <c r="I19" s="33">
+        <v>4561.53</v>
+      </c>
+      <c r="J19" s="44">
         <f>G19*I19</f>
-        <v>0</v>
-      </c>
-      <c r="K19" s="21"/>
-      <c r="M19" s="25"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="25"/>
-      <c r="S19" s="25"/>
-    </row>
-    <row r="20" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="18"/>
-      <c r="B20" s="37"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="41"/>
-      <c r="K20" s="21"/>
-      <c r="M20" s="25"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="25"/>
-      <c r="S20" s="25"/>
-    </row>
-    <row r="21" spans="1:19" ht="82.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="18">
-        <v>2</v>
-      </c>
-      <c r="B21" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="41"/>
-      <c r="K21" s="21"/>
-      <c r="M21" s="25"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="25"/>
-      <c r="S21" s="25"/>
-    </row>
-    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="18"/>
-      <c r="B22" s="37" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="36">
-        <v>1</v>
-      </c>
-      <c r="D22" s="38">
-        <f>D30</f>
-        <v>13.3</v>
-      </c>
-      <c r="E22" s="38">
-        <f>E30</f>
-        <v>1.7</v>
-      </c>
-      <c r="F22" s="38">
-        <v>0.15</v>
-      </c>
-      <c r="G22" s="39">
-        <f>PRODUCT(C22:F22)</f>
-        <v>3.3914999999999997</v>
-      </c>
-      <c r="H22" s="40"/>
-      <c r="I22" s="40"/>
-      <c r="J22" s="40"/>
+        <v>19575.805994999995</v>
+      </c>
+      <c r="K19" s="36"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A20" s="40"/>
+      <c r="B20" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="42"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="45">
+        <f>0.13*G19*(15452.6/5)</f>
+        <v>1724.1856553999996</v>
+      </c>
+      <c r="K20" s="36"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A21" s="40"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="45"/>
+      <c r="K21" s="36"/>
+    </row>
+    <row r="22" spans="1:19" ht="69" x14ac:dyDescent="0.3">
+      <c r="A22" s="18">
+        <v>3</v>
+      </c>
+      <c r="B22" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="19"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="41"/>
       <c r="K22" s="21"/>
       <c r="M22" s="25"/>
       <c r="N22" s="1"/>
@@ -9162,23 +9128,25 @@
     <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18"/>
       <c r="B23" s="37" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="C23" s="36">
         <v>1</v>
       </c>
       <c r="D23" s="38">
-        <v>10</v>
+        <f>D29</f>
+        <v>13.3</v>
       </c>
       <c r="E23" s="38">
-        <v>0.45</v>
+        <f>3.4/2</f>
+        <v>1.7</v>
       </c>
       <c r="F23" s="38">
-        <v>0.15</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="G23" s="39">
-        <f t="shared" ref="G23:G24" si="1">PRODUCT(C23:F23)</f>
-        <v>0.67499999999999993</v>
+        <f>PRODUCT(C23:F23)</f>
+        <v>1.6957499999999999</v>
       </c>
       <c r="H23" s="40"/>
       <c r="I23" s="40"/>
@@ -9199,17 +9167,18 @@
         <v>1</v>
       </c>
       <c r="D24" s="38">
-        <v>10</v>
+        <f>D23</f>
+        <v>13.3</v>
       </c>
       <c r="E24" s="38">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="F24" s="38">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="G24" s="39">
-        <f t="shared" si="1"/>
-        <v>0.89999999999999991</v>
+        <f>PRODUCT(C24:F24)</f>
+        <v>0.33250000000000002</v>
       </c>
       <c r="H24" s="40"/>
       <c r="I24" s="40"/>
@@ -9223,71 +9192,52 @@
       <c r="R24" s="25"/>
       <c r="S24" s="25"/>
     </row>
-    <row r="25" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="18"/>
+    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="40"/>
       <c r="B25" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25" s="36">
-        <v>0</v>
-      </c>
-      <c r="D25" s="38">
-        <f>D13</f>
-        <v>11.889667784212129</v>
-      </c>
-      <c r="E25" s="38">
-        <f>E13</f>
-        <v>1.3</v>
-      </c>
-      <c r="F25" s="38">
-        <v>0.15</v>
-      </c>
-      <c r="G25" s="39">
-        <f>PRODUCT(C25:F25)</f>
-        <v>0</v>
-      </c>
-      <c r="H25" s="40"/>
-      <c r="I25" s="40"/>
-      <c r="J25" s="40"/>
-      <c r="K25" s="21"/>
-      <c r="M25" s="25"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="1"/>
-      <c r="R25" s="25"/>
-      <c r="S25" s="25"/>
+        <v>40</v>
+      </c>
+      <c r="C25" s="42"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="33">
+        <f>SUM(G23:G24)</f>
+        <v>2.0282499999999999</v>
+      </c>
+      <c r="H25" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="I25" s="33">
+        <v>10634.5</v>
+      </c>
+      <c r="J25" s="44">
+        <f>G25*I25</f>
+        <v>21569.424625</v>
+      </c>
+      <c r="K25" s="36"/>
     </row>
     <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="40"/>
       <c r="B26" s="37" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C26" s="42"/>
       <c r="D26" s="43"/>
       <c r="E26" s="43"/>
       <c r="F26" s="43"/>
-      <c r="G26" s="33">
-        <f>SUM(G22:G25)</f>
-        <v>4.9664999999999999</v>
-      </c>
-      <c r="H26" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="I26" s="33">
-        <v>4561.53</v>
-      </c>
-      <c r="J26" s="44">
-        <f>G26*I26</f>
-        <v>22654.838744999997</v>
+      <c r="G26" s="43"/>
+      <c r="H26" s="43"/>
+      <c r="I26" s="43"/>
+      <c r="J26" s="45">
+        <f>0.13*G25*((114907.3+6135.3)/15)</f>
+        <v>2127.7069965666665</v>
       </c>
       <c r="K26" s="36"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="40"/>
-      <c r="B27" s="37" t="s">
-        <v>38</v>
-      </c>
+      <c r="B27" s="37"/>
       <c r="C27" s="42"/>
       <c r="D27" s="43"/>
       <c r="E27" s="43"/>
@@ -9295,40 +9245,52 @@
       <c r="G27" s="43"/>
       <c r="H27" s="43"/>
       <c r="I27" s="43"/>
-      <c r="J27" s="45">
-        <f>0.13*G26*(15452.6/5)</f>
-        <v>1995.3787854</v>
-      </c>
+      <c r="J27" s="45"/>
       <c r="K27" s="36"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A28" s="40"/>
-      <c r="B28" s="37"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
+    <row r="28" spans="1:19" s="1" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="63">
+        <v>4</v>
+      </c>
+      <c r="B28" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" s="64"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="39"/>
       <c r="J28" s="45"/>
-      <c r="K28" s="36"/>
-    </row>
-    <row r="29" spans="1:19" ht="69" x14ac:dyDescent="0.3">
-      <c r="A29" s="18">
-        <v>3</v>
-      </c>
-      <c r="B29" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="C29" s="19"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="41"/>
+      <c r="K28" s="29"/>
+    </row>
+    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="18"/>
+      <c r="B29" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="36">
+        <v>1</v>
+      </c>
+      <c r="D29" s="38">
+        <v>13.3</v>
+      </c>
+      <c r="E29" s="38">
+        <f>((1.7+0.5)/2)</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F29" s="38">
+        <f>3.5-0.15-0.075-0.05</f>
+        <v>3.2250000000000001</v>
+      </c>
+      <c r="G29" s="39">
+        <f>PRODUCT(C29:F29)</f>
+        <v>47.181750000000008</v>
+      </c>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
       <c r="K29" s="21"/>
       <c r="M29" s="25"/>
       <c r="N29" s="1"/>
@@ -9339,1428 +9301,666 @@
       <c r="S29" s="25"/>
     </row>
     <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="18"/>
+      <c r="A30" s="40"/>
       <c r="B30" s="37" t="s">
-        <v>50</v>
-      </c>
-      <c r="C30" s="36">
-        <v>1</v>
-      </c>
-      <c r="D30" s="38">
-        <f>D38</f>
-        <v>13.3</v>
-      </c>
-      <c r="E30" s="38">
-        <f>3.4/2</f>
-        <v>1.7</v>
-      </c>
-      <c r="F30" s="38">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="G30" s="39">
-        <f>PRODUCT(C30:F30)</f>
-        <v>1.6957499999999999</v>
-      </c>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
-      <c r="K30" s="21"/>
-      <c r="M30" s="25"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
-      <c r="P30" s="1"/>
-      <c r="Q30" s="1"/>
-      <c r="R30" s="25"/>
-      <c r="S30" s="25"/>
+        <v>40</v>
+      </c>
+      <c r="C30" s="42"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="33">
+        <f>SUM(G29:G29)</f>
+        <v>47.181750000000008</v>
+      </c>
+      <c r="H30" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="I30" s="33">
+        <v>9709.43</v>
+      </c>
+      <c r="J30" s="44">
+        <f>G30*I30</f>
+        <v>458107.89890250011</v>
+      </c>
+      <c r="K30" s="36"/>
     </row>
     <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="18"/>
-      <c r="B31" s="37"/>
-      <c r="C31" s="36">
-        <v>1</v>
-      </c>
-      <c r="D31" s="38">
-        <f>D30</f>
-        <v>13.3</v>
-      </c>
-      <c r="E31" s="38">
-        <v>0.5</v>
-      </c>
-      <c r="F31" s="38">
-        <v>0.05</v>
-      </c>
-      <c r="G31" s="39">
-        <f>PRODUCT(C31:F31)</f>
-        <v>0.33250000000000002</v>
-      </c>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="40"/>
-      <c r="K31" s="21"/>
-      <c r="M31" s="25"/>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
-      <c r="P31" s="1"/>
-      <c r="Q31" s="1"/>
-      <c r="R31" s="25"/>
-      <c r="S31" s="25"/>
-    </row>
-    <row r="32" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="18"/>
-      <c r="B32" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="C32" s="36">
-        <f>C25</f>
-        <v>0</v>
-      </c>
-      <c r="D32" s="38">
-        <f>D25</f>
-        <v>11.889667784212129</v>
-      </c>
-      <c r="E32" s="38">
-        <f>E25</f>
-        <v>1.3</v>
-      </c>
-      <c r="F32" s="38">
-        <v>0.05</v>
-      </c>
-      <c r="G32" s="39">
-        <f>0*PRODUCT(C32:F32)</f>
-        <v>0</v>
-      </c>
-      <c r="H32" s="40"/>
-      <c r="I32" s="40"/>
-      <c r="J32" s="40"/>
-      <c r="K32" s="21"/>
-      <c r="M32" s="25"/>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
-      <c r="P32" s="1"/>
-      <c r="Q32" s="1"/>
-      <c r="R32" s="25"/>
-      <c r="S32" s="25"/>
-    </row>
-    <row r="33" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="18"/>
-      <c r="B33" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="C33" s="36">
-        <v>1</v>
-      </c>
-      <c r="D33" s="38">
-        <f>D60</f>
-        <v>3.8860103626943006</v>
-      </c>
-      <c r="E33" s="38">
-        <v>0.23</v>
-      </c>
-      <c r="F33" s="38">
-        <v>0.05</v>
-      </c>
-      <c r="G33" s="39">
-        <f>0*PRODUCT(C33:F33)</f>
-        <v>0</v>
-      </c>
-      <c r="H33" s="40"/>
-      <c r="I33" s="40"/>
-      <c r="J33" s="40"/>
-      <c r="K33" s="21"/>
-      <c r="M33" s="25"/>
-      <c r="N33" s="1"/>
-      <c r="O33" s="1"/>
-      <c r="P33" s="1"/>
-      <c r="Q33" s="1"/>
-      <c r="R33" s="25"/>
-      <c r="S33" s="25"/>
+      <c r="A31" s="40"/>
+      <c r="B31" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="42"/>
+      <c r="D31" s="43"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="43"/>
+      <c r="H31" s="43"/>
+      <c r="I31" s="43"/>
+      <c r="J31" s="45">
+        <f>0.13*G30*((27092.1)/5)</f>
+        <v>33234.569918550005</v>
+      </c>
+      <c r="K31" s="36"/>
+    </row>
+    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="40"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="42"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="43"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="43"/>
+      <c r="J32" s="45"/>
+      <c r="K32" s="36"/>
+    </row>
+    <row r="33" spans="1:19" s="1" customFormat="1" ht="69" x14ac:dyDescent="0.3">
+      <c r="A33" s="63">
+        <v>5</v>
+      </c>
+      <c r="B33" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="67" t="s">
+        <v>70</v>
+      </c>
+      <c r="E33" s="67" t="s">
+        <v>71</v>
+      </c>
+      <c r="F33" s="67" t="s">
+        <v>72</v>
+      </c>
+      <c r="G33" s="39"/>
+      <c r="H33" s="39"/>
+      <c r="I33" s="39"/>
+      <c r="J33" s="45"/>
+      <c r="K33" s="29"/>
     </row>
     <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="40"/>
-      <c r="B34" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="C34" s="42"/>
-      <c r="D34" s="43"/>
-      <c r="E34" s="43"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="33">
-        <f>SUM(G30:G33)</f>
-        <v>2.0282499999999999</v>
-      </c>
-      <c r="H34" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="I34" s="33">
-        <v>10634.5</v>
-      </c>
-      <c r="J34" s="44">
-        <f>G34*I34</f>
-        <v>21569.424625</v>
-      </c>
+      <c r="B34" s="37" t="str">
+        <f>B30</f>
+        <v>Sub-total</v>
+      </c>
+      <c r="C34" s="42">
+        <f>TRUNC(D35/0.15,0)</f>
+        <v>62</v>
+      </c>
+      <c r="D34" s="43">
+        <f>0.6</f>
+        <v>0.6</v>
+      </c>
+      <c r="E34" s="43">
+        <f>10*10/162</f>
+        <v>0.61728395061728392</v>
+      </c>
+      <c r="F34" s="43">
+        <f>PRODUCT(C34:E34)</f>
+        <v>22.962962962962958</v>
+      </c>
+      <c r="G34" s="43">
+        <f>F34/1000</f>
+        <v>2.2962962962962959E-2</v>
+      </c>
+      <c r="H34" s="43"/>
+      <c r="I34" s="43"/>
+      <c r="J34" s="45"/>
       <c r="K34" s="36"/>
     </row>
-    <row r="35" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="40"/>
-      <c r="B35" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="C35" s="42"/>
-      <c r="D35" s="43"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="43"/>
-      <c r="H35" s="43"/>
-      <c r="I35" s="43"/>
-      <c r="J35" s="45">
-        <f>0.13*G34*((114907.3+6135.3)/15)</f>
-        <v>2127.7069965666665</v>
-      </c>
-      <c r="K35" s="36"/>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="42">
+        <f>TRUNC(D34/0.15,0)+1</f>
+        <v>5</v>
+      </c>
+      <c r="D35" s="68">
+        <f>10-0.6</f>
+        <v>9.4</v>
+      </c>
+      <c r="E35" s="43">
+        <f>10*10/162</f>
+        <v>0.61728395061728392</v>
+      </c>
+      <c r="F35" s="43">
+        <f>PRODUCT(C35:E35)</f>
+        <v>29.012345679012345</v>
+      </c>
+      <c r="G35" s="43">
+        <f>F35/1000</f>
+        <v>2.9012345679012345E-2</v>
+      </c>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="M35" s="69"/>
+      <c r="N35" s="69"/>
     </row>
     <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="40"/>
-      <c r="B36" s="37"/>
+      <c r="B36" s="37" t="s">
+        <v>40</v>
+      </c>
       <c r="C36" s="42"/>
       <c r="D36" s="43"/>
       <c r="E36" s="43"/>
       <c r="F36" s="43"/>
-      <c r="G36" s="43"/>
-      <c r="H36" s="43"/>
-      <c r="I36" s="43"/>
-      <c r="J36" s="45"/>
+      <c r="G36" s="33">
+        <f>SUM(G34:G35)</f>
+        <v>5.1975308641975304E-2</v>
+      </c>
+      <c r="H36" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="I36" s="33">
+        <v>124140</v>
+      </c>
+      <c r="J36" s="44">
+        <f>G36*I36</f>
+        <v>6452.2148148148144</v>
+      </c>
       <c r="K36" s="36"/>
     </row>
-    <row r="37" spans="1:19" s="1" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="63">
-        <v>4</v>
-      </c>
-      <c r="B37" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="C37" s="64"/>
-      <c r="D37" s="39"/>
-      <c r="E37" s="39"/>
-      <c r="F37" s="39"/>
-      <c r="G37" s="39"/>
-      <c r="H37" s="39"/>
-      <c r="I37" s="39"/>
-      <c r="J37" s="45"/>
-      <c r="K37" s="29"/>
-    </row>
-    <row r="38" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="18"/>
-      <c r="B38" s="37" t="s">
-        <v>50</v>
-      </c>
-      <c r="C38" s="36">
+    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="40"/>
+      <c r="B37" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" s="42"/>
+      <c r="D37" s="43"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="43"/>
+      <c r="G37" s="43"/>
+      <c r="H37" s="43"/>
+      <c r="I37" s="43"/>
+      <c r="J37" s="45">
+        <f>0.13*G36*110960</f>
+        <v>749.73343209876532</v>
+      </c>
+      <c r="K37" s="36"/>
+    </row>
+    <row r="38" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+    </row>
+    <row r="39" spans="1:19" s="1" customFormat="1" ht="69" x14ac:dyDescent="0.3">
+      <c r="A39" s="63">
+        <v>6</v>
+      </c>
+      <c r="B39" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" s="64"/>
+      <c r="D39" s="39"/>
+      <c r="E39" s="39"/>
+      <c r="F39" s="39"/>
+      <c r="G39" s="39"/>
+      <c r="H39" s="39"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="45"/>
+      <c r="K39" s="29"/>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A40" s="40"/>
+      <c r="B40" s="24" t="str">
+        <f>B30</f>
+        <v>Sub-total</v>
+      </c>
+      <c r="C40" s="42">
+        <f>1</f>
         <v>1</v>
       </c>
-      <c r="D38" s="38">
-        <v>13.3</v>
-      </c>
-      <c r="E38" s="38">
-        <f>((1.7+0.5)/2)</f>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F38" s="38">
-        <f>3.5-0.15-0.1-0.05</f>
-        <v>3.2</v>
-      </c>
-      <c r="G38" s="39">
-        <f>PRODUCT(C38:F38)</f>
-        <v>46.81600000000001</v>
-      </c>
-      <c r="H38" s="40"/>
-      <c r="I38" s="40"/>
-      <c r="J38" s="40"/>
-      <c r="K38" s="21"/>
-      <c r="M38" s="25"/>
-      <c r="N38" s="1"/>
-      <c r="O38" s="1"/>
-      <c r="P38" s="1"/>
-      <c r="Q38" s="1"/>
-      <c r="R38" s="25"/>
-      <c r="S38" s="25"/>
-    </row>
-    <row r="39" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="40"/>
-      <c r="B39" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="C39" s="42"/>
-      <c r="D39" s="43"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="43"/>
-      <c r="G39" s="33">
-        <f>SUM(G38:G38)</f>
-        <v>46.81600000000001</v>
-      </c>
-      <c r="H39" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="I39" s="33">
-        <v>9709.43</v>
-      </c>
-      <c r="J39" s="44">
-        <f>G39*I39</f>
-        <v>454556.67488000012</v>
-      </c>
-      <c r="K39" s="36"/>
-    </row>
-    <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="40"/>
-      <c r="B40" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="C40" s="42"/>
-      <c r="D40" s="43"/>
-      <c r="E40" s="43"/>
-      <c r="F40" s="43"/>
-      <c r="G40" s="43"/>
+      <c r="D40" s="43">
+        <v>10</v>
+      </c>
+      <c r="E40" s="43">
+        <v>0.6</v>
+      </c>
+      <c r="F40" s="43">
+        <v>0.15</v>
+      </c>
+      <c r="G40" s="39">
+        <f>PRODUCT(C40:F40)</f>
+        <v>0.89999999999999991</v>
+      </c>
       <c r="H40" s="43"/>
       <c r="I40" s="43"/>
-      <c r="J40" s="45">
-        <f>0.13*G39*((27092.1)/5)</f>
-        <v>32976.937593600007</v>
-      </c>
+      <c r="J40" s="45"/>
       <c r="K40" s="36"/>
     </row>
     <row r="41" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="40"/>
-      <c r="B41" s="37"/>
+      <c r="B41" s="37" t="s">
+        <v>40</v>
+      </c>
       <c r="C41" s="42"/>
       <c r="D41" s="43"/>
       <c r="E41" s="43"/>
       <c r="F41" s="43"/>
-      <c r="G41" s="43"/>
-      <c r="H41" s="43"/>
-      <c r="I41" s="43"/>
-      <c r="J41" s="45"/>
+      <c r="G41" s="33">
+        <f>SUM(G40:G40)</f>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="H41" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="I41" s="33">
+        <v>11588.17</v>
+      </c>
+      <c r="J41" s="44">
+        <f>G41*I41</f>
+        <v>10429.352999999999</v>
+      </c>
       <c r="K41" s="36"/>
     </row>
-    <row r="42" spans="1:19" s="1" customFormat="1" ht="69" x14ac:dyDescent="0.3">
-      <c r="A42" s="63">
-        <v>5</v>
-      </c>
-      <c r="B42" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="C42" s="64" t="s">
-        <v>7</v>
-      </c>
-      <c r="D42" s="67" t="s">
-        <v>70</v>
-      </c>
-      <c r="E42" s="67" t="s">
-        <v>71</v>
-      </c>
-      <c r="F42" s="67" t="s">
-        <v>72</v>
-      </c>
-      <c r="G42" s="39"/>
-      <c r="H42" s="39"/>
-      <c r="I42" s="39"/>
-      <c r="J42" s="45"/>
-      <c r="K42" s="29"/>
+    <row r="42" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="40"/>
+      <c r="B42" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" s="42"/>
+      <c r="D42" s="43"/>
+      <c r="E42" s="43"/>
+      <c r="F42" s="43"/>
+      <c r="G42" s="43"/>
+      <c r="H42" s="43"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="45">
+        <f>0.13*G41*((128662.2+6685.5)/15)</f>
+        <v>1055.7120600000001</v>
+      </c>
+      <c r="K42" s="36"/>
     </row>
     <row r="43" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="40"/>
-      <c r="B43" s="37" t="str">
-        <f>B39</f>
-        <v>Sub-total</v>
-      </c>
-      <c r="C43" s="42">
-        <f>TRUNC(D44/0.15,0)</f>
-        <v>62</v>
-      </c>
-      <c r="D43" s="43">
-        <f>0.6</f>
-        <v>0.6</v>
-      </c>
-      <c r="E43" s="43">
-        <f>10*10/162</f>
-        <v>0.61728395061728392</v>
-      </c>
-      <c r="F43" s="43">
-        <f>PRODUCT(C43:E43)</f>
-        <v>22.962962962962958</v>
-      </c>
-      <c r="G43" s="43">
-        <f>F43/1000</f>
-        <v>2.2962962962962959E-2</v>
-      </c>
+      <c r="B43" s="37"/>
+      <c r="C43" s="42"/>
+      <c r="D43" s="43"/>
+      <c r="E43" s="43"/>
+      <c r="F43" s="43"/>
+      <c r="G43" s="43"/>
       <c r="H43" s="43"/>
       <c r="I43" s="43"/>
       <c r="J43" s="45"/>
       <c r="K43" s="36"/>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="42">
-        <f>TRUNC(D43/0.15,0)+1</f>
-        <v>5</v>
-      </c>
-      <c r="D44" s="68">
-        <f>10-0.6</f>
-        <v>9.4</v>
-      </c>
-      <c r="E44" s="43">
-        <f>10*10/162</f>
-        <v>0.61728395061728392</v>
-      </c>
-      <c r="F44" s="43">
-        <f>PRODUCT(C44:E44)</f>
-        <v>29.012345679012345</v>
-      </c>
-      <c r="G44" s="43">
-        <f>F44/1000</f>
-        <v>2.9012345679012345E-2</v>
+    <row r="44" spans="1:19" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="18">
+        <v>7</v>
+      </c>
+      <c r="B44" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="C44" s="19">
+        <v>4</v>
+      </c>
+      <c r="D44" s="20">
+        <v>2.5</v>
+      </c>
+      <c r="E44" s="21"/>
+      <c r="F44" s="21"/>
+      <c r="G44" s="34">
+        <f>PRODUCT(C44:F44)</f>
+        <v>10</v>
       </c>
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
-      <c r="K44" s="5"/>
-      <c r="M44" s="69"/>
-      <c r="N44" s="69"/>
+      <c r="K44" s="21"/>
+      <c r="M44" s="25"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="1"/>
+      <c r="P44" s="1"/>
+      <c r="Q44" s="1"/>
+      <c r="R44" s="25"/>
+      <c r="S44" s="25"/>
     </row>
     <row r="45" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="40"/>
+      <c r="A45" s="18"/>
       <c r="B45" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="C45" s="42"/>
-      <c r="D45" s="43"/>
-      <c r="E45" s="43"/>
-      <c r="F45" s="43"/>
-      <c r="G45" s="33">
-        <f>SUM(G43:G44)</f>
-        <v>5.1975308641975304E-2</v>
-      </c>
-      <c r="H45" s="33" t="s">
-        <v>73</v>
-      </c>
-      <c r="I45" s="33">
-        <v>124140</v>
-      </c>
-      <c r="J45" s="44">
+      <c r="C45" s="36"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="38"/>
+      <c r="F45" s="38"/>
+      <c r="G45" s="34">
+        <f>SUM(G44)</f>
+        <v>10</v>
+      </c>
+      <c r="H45" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="I45" s="23">
+        <v>5144.96</v>
+      </c>
+      <c r="J45" s="34">
         <f>G45*I45</f>
-        <v>6452.2148148148144</v>
-      </c>
-      <c r="K45" s="36"/>
+        <v>51449.599999999999</v>
+      </c>
+      <c r="K45" s="21"/>
+      <c r="M45" s="25"/>
+      <c r="N45" s="1"/>
+      <c r="O45" s="1"/>
+      <c r="P45" s="1"/>
+      <c r="Q45" s="1"/>
+      <c r="R45" s="25"/>
+      <c r="S45" s="25"/>
     </row>
     <row r="46" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="40"/>
+      <c r="A46" s="18"/>
       <c r="B46" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="C46" s="42"/>
-      <c r="D46" s="43"/>
-      <c r="E46" s="43"/>
-      <c r="F46" s="43"/>
-      <c r="G46" s="43"/>
-      <c r="H46" s="43"/>
-      <c r="I46" s="43"/>
+      <c r="C46" s="36"/>
+      <c r="D46" s="38"/>
+      <c r="E46" s="38"/>
+      <c r="F46" s="38"/>
+      <c r="G46" s="39"/>
+      <c r="H46" s="40"/>
+      <c r="I46" s="40"/>
       <c r="J46" s="45">
-        <f>0.13*G45*110960</f>
-        <v>749.73343209876532</v>
-      </c>
-      <c r="K46" s="36"/>
-    </row>
-    <row r="47" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
-      <c r="I47" s="5"/>
-      <c r="J47" s="5"/>
-      <c r="K47" s="5"/>
-    </row>
-    <row r="48" spans="1:19" s="1" customFormat="1" ht="69" x14ac:dyDescent="0.3">
-      <c r="A48" s="63">
-        <v>6</v>
+        <f>0.13*G45*57364.6/12.5</f>
+        <v>5965.9183999999996</v>
+      </c>
+      <c r="K46" s="21"/>
+      <c r="M46" s="25"/>
+      <c r="N46" s="1"/>
+      <c r="O46" s="1"/>
+      <c r="P46" s="1"/>
+      <c r="Q46" s="1"/>
+      <c r="R46" s="25"/>
+      <c r="S46" s="25"/>
+    </row>
+    <row r="47" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="40"/>
+      <c r="B47" s="37"/>
+      <c r="C47" s="42"/>
+      <c r="D47" s="43"/>
+      <c r="E47" s="43"/>
+      <c r="F47" s="43"/>
+      <c r="G47" s="43"/>
+      <c r="H47" s="43"/>
+      <c r="I47" s="43"/>
+      <c r="J47" s="45"/>
+      <c r="K47" s="36"/>
+    </row>
+    <row r="48" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="18">
+        <v>8</v>
       </c>
       <c r="B48" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="C48" s="64"/>
-      <c r="D48" s="39"/>
-      <c r="E48" s="39"/>
-      <c r="F48" s="39"/>
-      <c r="G48" s="39"/>
-      <c r="H48" s="39"/>
-      <c r="I48" s="39"/>
-      <c r="J48" s="45"/>
-      <c r="K48" s="29"/>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A49" s="40"/>
-      <c r="B49" s="24" t="str">
-        <f>B39</f>
-        <v>Sub-total</v>
-      </c>
-      <c r="C49" s="42">
-        <f>1</f>
+        <v>30</v>
+      </c>
+      <c r="C48" s="19">
         <v>1</v>
       </c>
-      <c r="D49" s="43">
-        <v>10</v>
-      </c>
-      <c r="E49" s="43">
-        <v>0.6</v>
-      </c>
-      <c r="F49" s="43">
-        <v>0.15</v>
-      </c>
-      <c r="G49" s="39">
-        <f>PRODUCT(C49:F49)</f>
-        <v>0.89999999999999991</v>
-      </c>
-      <c r="H49" s="43"/>
-      <c r="I49" s="43"/>
-      <c r="J49" s="45"/>
-      <c r="K49" s="36"/>
-    </row>
-    <row r="50" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="40"/>
-      <c r="B50" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="C50" s="42"/>
-      <c r="D50" s="43"/>
-      <c r="E50" s="43"/>
-      <c r="F50" s="43"/>
-      <c r="G50" s="33">
-        <f>SUM(G49:G49)</f>
-        <v>0.89999999999999991</v>
-      </c>
-      <c r="H50" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="I50" s="33">
-        <v>11588.17</v>
-      </c>
-      <c r="J50" s="44">
-        <f>G50*I50</f>
-        <v>10429.352999999999</v>
-      </c>
-      <c r="K50" s="36"/>
-    </row>
-    <row r="51" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="40"/>
-      <c r="B51" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="C51" s="42"/>
-      <c r="D51" s="43"/>
-      <c r="E51" s="43"/>
-      <c r="F51" s="43"/>
-      <c r="G51" s="43"/>
-      <c r="H51" s="43"/>
-      <c r="I51" s="43"/>
-      <c r="J51" s="45">
-        <f>0.13*G50*((128662.2+6685.5)/15)</f>
-        <v>1055.7120600000001</v>
-      </c>
-      <c r="K51" s="36"/>
-    </row>
-    <row r="52" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="40"/>
-      <c r="B52" s="37"/>
-      <c r="C52" s="42"/>
-      <c r="D52" s="43"/>
-      <c r="E52" s="43"/>
-      <c r="F52" s="43"/>
-      <c r="G52" s="43"/>
-      <c r="H52" s="43"/>
-      <c r="I52" s="43"/>
-      <c r="J52" s="45"/>
-      <c r="K52" s="36"/>
-    </row>
-    <row r="53" spans="1:19" ht="82.8" x14ac:dyDescent="0.3">
-      <c r="A53" s="18">
-        <v>7</v>
-      </c>
-      <c r="B53" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="C53" s="19">
-        <v>4</v>
-      </c>
-      <c r="D53" s="20">
-        <v>2.5</v>
-      </c>
-      <c r="E53" s="21"/>
-      <c r="F53" s="21"/>
-      <c r="G53" s="34">
-        <f>PRODUCT(C53:F53)</f>
-        <v>10</v>
-      </c>
-      <c r="H53" s="5"/>
-      <c r="I53" s="5"/>
-      <c r="J53" s="5"/>
-      <c r="K53" s="21"/>
-      <c r="M53" s="25"/>
-      <c r="N53" s="1"/>
-      <c r="O53" s="1"/>
-      <c r="P53" s="1"/>
-      <c r="Q53" s="1"/>
-      <c r="R53" s="25"/>
-      <c r="S53" s="25"/>
-    </row>
-    <row r="54" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="18"/>
-      <c r="B54" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="C54" s="36"/>
-      <c r="D54" s="38"/>
-      <c r="E54" s="38"/>
-      <c r="F54" s="38"/>
-      <c r="G54" s="34">
-        <f>SUM(G53)</f>
-        <v>10</v>
-      </c>
-      <c r="H54" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="I54" s="23">
-        <v>5144.96</v>
-      </c>
-      <c r="J54" s="34">
-        <f>G54*I54</f>
-        <v>51449.599999999999</v>
-      </c>
-      <c r="K54" s="21"/>
-      <c r="M54" s="25"/>
-      <c r="N54" s="1"/>
-      <c r="O54" s="1"/>
-      <c r="P54" s="1"/>
-      <c r="Q54" s="1"/>
-      <c r="R54" s="25"/>
-      <c r="S54" s="25"/>
-    </row>
-    <row r="55" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="18"/>
-      <c r="B55" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="C55" s="36"/>
-      <c r="D55" s="38"/>
-      <c r="E55" s="38"/>
-      <c r="F55" s="38"/>
-      <c r="G55" s="39"/>
-      <c r="H55" s="40"/>
-      <c r="I55" s="40"/>
-      <c r="J55" s="45">
-        <f>0.13*G54*57364.6/12.5</f>
-        <v>5965.9183999999996</v>
-      </c>
-      <c r="K55" s="21"/>
-      <c r="M55" s="25"/>
-      <c r="N55" s="1"/>
-      <c r="O55" s="1"/>
-      <c r="P55" s="1"/>
-      <c r="Q55" s="1"/>
-      <c r="R55" s="25"/>
-      <c r="S55" s="25"/>
-    </row>
-    <row r="56" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="40"/>
-      <c r="B56" s="37"/>
-      <c r="C56" s="42"/>
-      <c r="D56" s="43"/>
-      <c r="E56" s="43"/>
-      <c r="F56" s="43"/>
-      <c r="G56" s="43"/>
-      <c r="H56" s="43"/>
-      <c r="I56" s="43"/>
-      <c r="J56" s="45"/>
-      <c r="K56" s="36"/>
-    </row>
-    <row r="57" spans="1:19" ht="30.6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="40">
-        <v>6</v>
-      </c>
-      <c r="B57" s="65" t="s">
-        <v>56</v>
-      </c>
-      <c r="C57" s="42"/>
-      <c r="D57" s="43"/>
-      <c r="E57" s="43"/>
-      <c r="F57" s="43"/>
-      <c r="G57" s="43"/>
-      <c r="H57" s="43"/>
-      <c r="I57" s="43"/>
-      <c r="J57" s="45"/>
-      <c r="K57" s="36"/>
-    </row>
-    <row r="58" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="18"/>
-      <c r="B58" s="37" t="s">
-        <v>50</v>
-      </c>
-      <c r="C58" s="36">
+      <c r="D48" s="20"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="34">
+        <f t="shared" ref="G48" si="2">PRODUCT(C48:F48)</f>
         <v>1</v>
       </c>
-      <c r="D58" s="38">
-        <f>(11.17+11.17+12.333+4.42)/3.281</f>
-        <v>11.914964949710455</v>
-      </c>
-      <c r="E58" s="38">
-        <v>0.23</v>
-      </c>
-      <c r="F58" s="38">
-        <v>0.45</v>
-      </c>
-      <c r="G58" s="39">
-        <f>PRODUCT(C58:F58)</f>
-        <v>1.2331988722950322</v>
-      </c>
-      <c r="H58" s="40"/>
-      <c r="I58" s="40"/>
-      <c r="J58" s="40"/>
-      <c r="K58" s="21"/>
-      <c r="M58" s="25"/>
-      <c r="N58" s="1"/>
-      <c r="O58" s="1"/>
-      <c r="P58" s="1"/>
-      <c r="Q58" s="1"/>
-      <c r="R58" s="25"/>
-      <c r="S58" s="25"/>
-    </row>
-    <row r="59" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="18"/>
-      <c r="B59" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="C59" s="36">
-        <f>31</f>
+      <c r="H48" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D59" s="38">
-        <f>1.3-0.23</f>
-        <v>1.07</v>
-      </c>
-      <c r="E59" s="38">
-        <v>0.15</v>
-      </c>
-      <c r="F59" s="38">
-        <v>0.15</v>
-      </c>
-      <c r="G59" s="39">
-        <f>PRODUCT(C59:F59)</f>
-        <v>0.74632500000000002</v>
-      </c>
-      <c r="H59" s="40"/>
-      <c r="I59" s="40"/>
-      <c r="J59" s="40"/>
-      <c r="K59" s="21"/>
-      <c r="M59" s="25"/>
-      <c r="N59" s="1"/>
-      <c r="O59" s="1"/>
-      <c r="P59" s="1"/>
-      <c r="Q59" s="1"/>
-      <c r="R59" s="25"/>
-      <c r="S59" s="25"/>
-    </row>
-    <row r="60" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="18"/>
-      <c r="B60" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="C60" s="36">
-        <v>1</v>
-      </c>
-      <c r="D60" s="38">
-        <f>12.75/3.281</f>
-        <v>3.8860103626943006</v>
-      </c>
-      <c r="E60" s="38">
-        <v>0.23</v>
-      </c>
-      <c r="F60" s="38">
-        <v>0.6</v>
-      </c>
-      <c r="G60" s="39">
-        <f>PRODUCT(C60:F60)</f>
-        <v>0.53626943005181349</v>
-      </c>
-      <c r="H60" s="40"/>
-      <c r="I60" s="40"/>
-      <c r="J60" s="40"/>
-      <c r="K60" s="21"/>
-      <c r="M60" s="25"/>
-      <c r="N60" s="1"/>
-      <c r="O60" s="1"/>
-      <c r="P60" s="1"/>
-      <c r="Q60" s="1"/>
-      <c r="R60" s="25"/>
-      <c r="S60" s="25"/>
-    </row>
-    <row r="61" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="40"/>
-      <c r="B61" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="C61" s="42"/>
-      <c r="D61" s="43"/>
-      <c r="E61" s="43"/>
-      <c r="F61" s="43"/>
-      <c r="G61" s="33">
-        <f>0*SUM(G58:G60)</f>
-        <v>0</v>
-      </c>
-      <c r="H61" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="I61" s="33">
-        <v>14362.76</v>
-      </c>
-      <c r="J61" s="44">
-        <f>G61*I61</f>
-        <v>0</v>
-      </c>
-      <c r="K61" s="36"/>
-    </row>
-    <row r="62" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="40"/>
-      <c r="B62" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="C62" s="42"/>
-      <c r="D62" s="43"/>
-      <c r="E62" s="43"/>
-      <c r="F62" s="43"/>
-      <c r="G62" s="43"/>
-      <c r="H62" s="43"/>
-      <c r="I62" s="43"/>
-      <c r="J62" s="45">
-        <f>0.13*G61*10311.74</f>
-        <v>0</v>
-      </c>
-      <c r="K62" s="36"/>
-    </row>
-    <row r="63" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="40"/>
-      <c r="B63" s="37"/>
-      <c r="C63" s="42"/>
-      <c r="D63" s="43"/>
-      <c r="E63" s="43"/>
-      <c r="F63" s="43"/>
-      <c r="G63" s="43"/>
-      <c r="H63" s="43"/>
-      <c r="I63" s="43"/>
-      <c r="J63" s="45"/>
-      <c r="K63" s="36"/>
-    </row>
-    <row r="64" spans="1:19" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="40">
-        <v>7</v>
-      </c>
-      <c r="B64" s="65" t="s">
-        <v>58</v>
-      </c>
-      <c r="C64" s="42"/>
-      <c r="D64" s="43"/>
-      <c r="E64" s="43"/>
-      <c r="F64" s="43"/>
-      <c r="G64" s="43"/>
-      <c r="H64" s="43"/>
-      <c r="I64" s="43"/>
-      <c r="J64" s="45"/>
-      <c r="K64" s="36"/>
-    </row>
-    <row r="65" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="18"/>
-      <c r="B65" s="37" t="s">
-        <v>60</v>
-      </c>
-      <c r="C65" s="36">
-        <v>1</v>
-      </c>
-      <c r="D65" s="38">
-        <f>21.9+3.04</f>
-        <v>24.939999999999998</v>
-      </c>
-      <c r="E65" s="38">
-        <v>0.3</v>
-      </c>
-      <c r="F65" s="38"/>
-      <c r="G65" s="39">
-        <f>PRODUCT(C65:F65)</f>
-        <v>7.4819999999999993</v>
-      </c>
-      <c r="H65" s="40"/>
-      <c r="I65" s="40"/>
-      <c r="J65" s="40"/>
-      <c r="K65" s="21"/>
-      <c r="M65" s="25"/>
-      <c r="N65" s="1"/>
-      <c r="O65" s="1"/>
-      <c r="P65" s="1"/>
-      <c r="Q65" s="1"/>
-      <c r="R65" s="25"/>
-      <c r="S65" s="25"/>
-    </row>
-    <row r="66" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="18"/>
-      <c r="B66" s="37"/>
-      <c r="C66" s="36">
-        <v>1</v>
-      </c>
-      <c r="D66" s="38">
-        <f>13.917/3.281</f>
-        <v>4.2416946053032607</v>
-      </c>
-      <c r="E66" s="38">
-        <f>51.083/3.281</f>
-        <v>15.569338616275525</v>
-      </c>
-      <c r="F66" s="38"/>
-      <c r="G66" s="39">
-        <f>PRODUCT(C66:F66)</f>
-        <v>66.040379616795633</v>
-      </c>
-      <c r="H66" s="40"/>
-      <c r="I66" s="40"/>
-      <c r="J66" s="40"/>
-      <c r="K66" s="21"/>
-      <c r="M66" s="25"/>
-      <c r="N66" s="1"/>
-      <c r="O66" s="1"/>
-      <c r="P66" s="1"/>
-      <c r="Q66" s="1"/>
-      <c r="R66" s="25"/>
-      <c r="S66" s="25"/>
-    </row>
-    <row r="67" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="18"/>
-      <c r="B67" s="37"/>
-      <c r="C67" s="36">
-        <v>1</v>
-      </c>
-      <c r="D67" s="38">
-        <f>22.17/3.281</f>
-        <v>6.7570862541907957</v>
-      </c>
-      <c r="E67" s="38">
-        <f>12.5/3.281</f>
-        <v>3.8098140810728434</v>
-      </c>
-      <c r="F67" s="38"/>
-      <c r="G67" s="39">
-        <f>PRODUCT(C67:F67)</f>
-        <v>25.743242358239847</v>
-      </c>
-      <c r="H67" s="40"/>
-      <c r="I67" s="40"/>
-      <c r="J67" s="40"/>
-      <c r="K67" s="21"/>
-      <c r="M67" s="25"/>
-      <c r="N67" s="1"/>
-      <c r="O67" s="1"/>
-      <c r="P67" s="1"/>
-      <c r="Q67" s="1"/>
-      <c r="R67" s="25"/>
-      <c r="S67" s="25"/>
-    </row>
-    <row r="68" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="40"/>
-      <c r="B68" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="C68" s="42"/>
-      <c r="D68" s="43"/>
-      <c r="E68" s="43"/>
-      <c r="F68" s="43"/>
-      <c r="G68" s="33">
-        <f>0*SUM(G65:G67)</f>
-        <v>0</v>
-      </c>
-      <c r="H68" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="I68" s="33">
-        <f>35*10.7639</f>
-        <v>376.73649999999998</v>
-      </c>
-      <c r="J68" s="44">
-        <f>G68*I68</f>
-        <v>0</v>
-      </c>
-      <c r="K68" s="36"/>
-    </row>
-    <row r="69" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="40"/>
-      <c r="B69" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="C69" s="42"/>
-      <c r="D69" s="43"/>
-      <c r="E69" s="43"/>
-      <c r="F69" s="43"/>
-      <c r="G69" s="43"/>
-      <c r="H69" s="43"/>
-      <c r="I69" s="43"/>
-      <c r="J69" s="45">
-        <f>0.13*J68</f>
-        <v>0</v>
-      </c>
-      <c r="K69" s="36"/>
-    </row>
-    <row r="70" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="40"/>
-      <c r="B70" s="37"/>
-      <c r="C70" s="42"/>
-      <c r="D70" s="43"/>
-      <c r="E70" s="43"/>
-      <c r="F70" s="43"/>
-      <c r="G70" s="43"/>
-      <c r="H70" s="43"/>
-      <c r="I70" s="43"/>
-      <c r="J70" s="45"/>
-      <c r="K70" s="36"/>
-    </row>
-    <row r="71" spans="1:19" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="40">
-        <v>8</v>
-      </c>
-      <c r="B71" s="65" t="s">
-        <v>61</v>
-      </c>
-      <c r="C71" s="42"/>
-      <c r="D71" s="43"/>
-      <c r="E71" s="43"/>
-      <c r="F71" s="43"/>
-      <c r="G71" s="43"/>
-      <c r="H71" s="43"/>
-      <c r="I71" s="43"/>
-      <c r="J71" s="45"/>
-      <c r="K71" s="36"/>
-    </row>
-    <row r="72" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="18"/>
-      <c r="B72" s="37" t="s">
-        <v>60</v>
-      </c>
-      <c r="C72" s="36">
-        <v>1</v>
-      </c>
-      <c r="D72" s="38">
-        <f>21.9+3.04</f>
-        <v>24.939999999999998</v>
-      </c>
-      <c r="E72" s="38">
-        <v>0.3</v>
-      </c>
-      <c r="F72" s="38"/>
-      <c r="G72" s="39">
-        <f>PRODUCT(C72:F72)</f>
-        <v>7.4819999999999993</v>
-      </c>
-      <c r="H72" s="40"/>
-      <c r="I72" s="40"/>
-      <c r="J72" s="40"/>
-      <c r="K72" s="21"/>
-      <c r="M72" s="25"/>
-      <c r="N72" s="1"/>
-      <c r="O72" s="1"/>
-      <c r="P72" s="1"/>
-      <c r="Q72" s="1"/>
-      <c r="R72" s="25"/>
-      <c r="S72" s="25"/>
-    </row>
-    <row r="73" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="18"/>
-      <c r="B73" s="37"/>
-      <c r="C73" s="36">
-        <v>1</v>
-      </c>
-      <c r="D73" s="38">
-        <f>13.917/3.281</f>
-        <v>4.2416946053032607</v>
-      </c>
-      <c r="E73" s="38">
-        <f>51.083/3.281</f>
-        <v>15.569338616275525</v>
-      </c>
-      <c r="F73" s="38"/>
-      <c r="G73" s="39">
-        <f>PRODUCT(C73:F73)</f>
-        <v>66.040379616795633</v>
-      </c>
-      <c r="H73" s="40"/>
-      <c r="I73" s="40"/>
-      <c r="J73" s="40"/>
-      <c r="K73" s="21"/>
-      <c r="M73" s="25"/>
-      <c r="N73" s="1"/>
-      <c r="O73" s="1"/>
-      <c r="P73" s="1"/>
-      <c r="Q73" s="1"/>
-      <c r="R73" s="25"/>
-      <c r="S73" s="25"/>
-    </row>
-    <row r="74" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="18"/>
-      <c r="B74" s="37"/>
-      <c r="C74" s="36">
-        <v>1</v>
-      </c>
-      <c r="D74" s="38">
-        <f>22.17/3.281</f>
-        <v>6.7570862541907957</v>
-      </c>
-      <c r="E74" s="38">
-        <f>12.5/3.281</f>
-        <v>3.8098140810728434</v>
-      </c>
-      <c r="F74" s="38"/>
-      <c r="G74" s="39">
-        <f>PRODUCT(C74:F74)</f>
-        <v>25.743242358239847</v>
-      </c>
-      <c r="H74" s="40"/>
-      <c r="I74" s="40"/>
-      <c r="J74" s="40"/>
-      <c r="K74" s="21"/>
-      <c r="M74" s="25"/>
-      <c r="N74" s="1"/>
-      <c r="O74" s="1"/>
-      <c r="P74" s="1"/>
-      <c r="Q74" s="1"/>
-      <c r="R74" s="25"/>
-      <c r="S74" s="25"/>
-    </row>
-    <row r="75" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="40"/>
-      <c r="B75" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="C75" s="42"/>
-      <c r="D75" s="43"/>
-      <c r="E75" s="43"/>
-      <c r="F75" s="43"/>
-      <c r="G75" s="33">
-        <f>0*SUM(G72:G74)</f>
-        <v>0</v>
-      </c>
-      <c r="H75" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="I75" s="33">
-        <f>23*10.7639</f>
-        <v>247.56969999999998</v>
-      </c>
-      <c r="J75" s="44">
-        <f>G75*I75</f>
-        <v>0</v>
-      </c>
-      <c r="K75" s="36"/>
-    </row>
-    <row r="76" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="40"/>
-      <c r="B76" s="37"/>
-      <c r="C76" s="42"/>
-      <c r="D76" s="43"/>
-      <c r="E76" s="43"/>
-      <c r="F76" s="43"/>
-      <c r="G76" s="33"/>
-      <c r="H76" s="33"/>
-      <c r="I76" s="33"/>
-      <c r="J76" s="44"/>
-      <c r="K76" s="36"/>
-    </row>
-    <row r="77" spans="1:19" ht="28.2" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="40">
-        <v>9</v>
-      </c>
-      <c r="B77" s="66" t="s">
-        <v>64</v>
-      </c>
-      <c r="C77" s="19">
-        <v>1</v>
-      </c>
-      <c r="D77" s="20"/>
-      <c r="E77" s="21"/>
-      <c r="F77" s="21"/>
-      <c r="G77" s="34">
-        <f>0*PRODUCT(C77:F77)</f>
-        <v>0</v>
-      </c>
-      <c r="H77" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="I77" s="23">
-        <v>20000</v>
-      </c>
-      <c r="J77" s="34">
-        <f>G77*I77</f>
-        <v>0</v>
-      </c>
-      <c r="K77" s="36"/>
-    </row>
-    <row r="78" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="40"/>
-      <c r="B78" s="37"/>
-      <c r="C78" s="42"/>
-      <c r="D78" s="43"/>
-      <c r="E78" s="43"/>
-      <c r="F78" s="43"/>
-      <c r="G78" s="33"/>
-      <c r="H78" s="33"/>
-      <c r="I78" s="33"/>
-      <c r="J78" s="44"/>
-      <c r="K78" s="36"/>
-    </row>
-    <row r="79" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="40"/>
-      <c r="B79" s="37"/>
-      <c r="C79" s="42"/>
-      <c r="D79" s="43"/>
-      <c r="E79" s="43"/>
-      <c r="F79" s="43"/>
-      <c r="G79" s="33"/>
-      <c r="H79" s="33"/>
-      <c r="I79" s="33"/>
-      <c r="J79" s="44"/>
-      <c r="K79" s="36"/>
-    </row>
-    <row r="80" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="18">
-        <v>8</v>
-      </c>
-      <c r="B80" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="C80" s="19">
-        <v>1</v>
-      </c>
-      <c r="D80" s="20"/>
-      <c r="E80" s="21"/>
-      <c r="F80" s="21"/>
-      <c r="G80" s="34">
-        <f t="shared" ref="G80" si="2">PRODUCT(C80:F80)</f>
-        <v>1</v>
-      </c>
-      <c r="H80" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="I80" s="23">
+      <c r="I48" s="23">
         <v>500</v>
       </c>
-      <c r="J80" s="34">
-        <f>G80*I80</f>
+      <c r="J48" s="34">
+        <f>G48*I48</f>
         <v>500</v>
       </c>
-      <c r="K80" s="21"/>
-      <c r="M80" s="25"/>
-      <c r="N80" s="1"/>
-      <c r="O80" s="1"/>
-      <c r="P80" s="1"/>
-      <c r="Q80" s="1"/>
-      <c r="R80" s="25"/>
-      <c r="S80" s="25"/>
-    </row>
-    <row r="81" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="18"/>
-      <c r="B81" s="24"/>
-      <c r="C81" s="19"/>
-      <c r="D81" s="20"/>
-      <c r="E81" s="21"/>
-      <c r="F81" s="21"/>
-      <c r="G81" s="23"/>
-      <c r="H81" s="22"/>
-      <c r="I81" s="23"/>
-      <c r="J81" s="41"/>
-      <c r="K81" s="21"/>
-      <c r="M81" s="25"/>
-      <c r="N81" s="1">
+      <c r="K48" s="21"/>
+      <c r="M48" s="25"/>
+      <c r="N48" s="1"/>
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
+      <c r="Q48" s="1"/>
+      <c r="R48" s="25"/>
+      <c r="S48" s="25"/>
+    </row>
+    <row r="49" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="18"/>
+      <c r="B49" s="24"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="23"/>
+      <c r="H49" s="22"/>
+      <c r="I49" s="23"/>
+      <c r="J49" s="41"/>
+      <c r="K49" s="21"/>
+      <c r="M49" s="25"/>
+      <c r="N49" s="1">
         <f>2.4*3.281</f>
         <v>7.8743999999999996</v>
       </c>
-      <c r="O81" s="1"/>
-      <c r="P81" s="1"/>
-      <c r="Q81" s="1"/>
-      <c r="R81" s="25"/>
-      <c r="S81" s="25"/>
-    </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A82" s="40"/>
-      <c r="B82" s="46" t="s">
+      <c r="O49" s="1"/>
+      <c r="P49" s="1"/>
+      <c r="Q49" s="1"/>
+      <c r="R49" s="25"/>
+      <c r="S49" s="25"/>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A50" s="40"/>
+      <c r="B50" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="C82" s="47"/>
-      <c r="D82" s="38"/>
-      <c r="E82" s="38"/>
-      <c r="F82" s="38"/>
-      <c r="G82" s="41"/>
-      <c r="H82" s="41"/>
-      <c r="I82" s="41"/>
-      <c r="J82" s="41">
-        <f>SUM(J10:J80)</f>
-        <v>614393.61235914705</v>
-      </c>
-      <c r="K82" s="36"/>
-    </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A83" s="58"/>
-      <c r="B83" s="61"/>
-      <c r="C83" s="62"/>
-      <c r="D83" s="59"/>
-      <c r="E83" s="59"/>
-      <c r="F83" s="59"/>
-      <c r="G83" s="60"/>
-      <c r="H83" s="60"/>
-      <c r="I83" s="60"/>
-      <c r="J83" s="60"/>
-      <c r="K83" s="57"/>
-    </row>
-    <row r="84" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="50"/>
-      <c r="B84" s="29" t="s">
+      <c r="C50" s="47"/>
+      <c r="D50" s="38"/>
+      <c r="E50" s="38"/>
+      <c r="F50" s="38"/>
+      <c r="G50" s="41"/>
+      <c r="H50" s="41"/>
+      <c r="I50" s="41"/>
+      <c r="J50" s="41">
+        <f>SUM(J10:J48)</f>
+        <v>614864.14527368033</v>
+      </c>
+      <c r="K50" s="36"/>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A51" s="58"/>
+      <c r="B51" s="61"/>
+      <c r="C51" s="62"/>
+      <c r="D51" s="59"/>
+      <c r="E51" s="59"/>
+      <c r="F51" s="59"/>
+      <c r="G51" s="60"/>
+      <c r="H51" s="60"/>
+      <c r="I51" s="60"/>
+      <c r="J51" s="60"/>
+      <c r="K51" s="57"/>
+    </row>
+    <row r="52" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="50"/>
+      <c r="B52" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="C84" s="88">
-        <f>J82</f>
-        <v>614393.61235914705</v>
-      </c>
-      <c r="D84" s="88"/>
-      <c r="E84" s="39">
+      <c r="C52" s="71">
+        <f>J50</f>
+        <v>614864.14527368033</v>
+      </c>
+      <c r="D52" s="71"/>
+      <c r="E52" s="39">
         <v>100</v>
       </c>
-      <c r="F84" s="51"/>
-      <c r="G84" s="52"/>
-      <c r="H84" s="51"/>
-      <c r="I84" s="53"/>
-      <c r="J84" s="54"/>
-      <c r="K84" s="55"/>
-    </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A85" s="56"/>
-      <c r="B85" s="29" t="s">
+      <c r="F52" s="51"/>
+      <c r="G52" s="52"/>
+      <c r="H52" s="51"/>
+      <c r="I52" s="53"/>
+      <c r="J52" s="54"/>
+      <c r="K52" s="55"/>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A53" s="56"/>
+      <c r="B53" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C85" s="91">
+      <c r="C53" s="74">
         <f>500000+86000</f>
         <v>586000</v>
       </c>
-      <c r="D85" s="91"/>
-      <c r="E85" s="39"/>
-      <c r="F85" s="49"/>
-      <c r="G85" s="48"/>
-      <c r="H85" s="48"/>
-      <c r="I85" s="48"/>
-      <c r="J85" s="48"/>
-      <c r="K85" s="49"/>
-    </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A86" s="56"/>
-      <c r="B86" s="29" t="s">
+      <c r="D53" s="74"/>
+      <c r="E53" s="39"/>
+      <c r="F53" s="49"/>
+      <c r="G53" s="48"/>
+      <c r="H53" s="48"/>
+      <c r="I53" s="48"/>
+      <c r="J53" s="48"/>
+      <c r="K53" s="49"/>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A54" s="56"/>
+      <c r="B54" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C86" s="91">
-        <f>C85-C88-C89</f>
+      <c r="C54" s="74">
+        <f>C53-C56-C57</f>
         <v>556700</v>
       </c>
-      <c r="D86" s="91"/>
-      <c r="E86" s="39">
-        <f>C86/C84*100</f>
-        <v>90.609665986334846</v>
-      </c>
-      <c r="F86" s="49"/>
-      <c r="G86" s="48"/>
-      <c r="H86" s="48"/>
-      <c r="I86" s="48"/>
-      <c r="J86" s="48"/>
-      <c r="K86" s="49"/>
-    </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A87" s="56"/>
-      <c r="B87" s="29" t="s">
+      <c r="D54" s="74"/>
+      <c r="E54" s="39">
+        <f>C54/C52*100</f>
+        <v>90.540325741747225</v>
+      </c>
+      <c r="F54" s="49"/>
+      <c r="G54" s="48"/>
+      <c r="H54" s="48"/>
+      <c r="I54" s="48"/>
+      <c r="J54" s="48"/>
+      <c r="K54" s="49"/>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A55" s="56"/>
+      <c r="B55" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C87" s="88">
-        <f>C84-C86</f>
-        <v>57693.612359147053</v>
-      </c>
-      <c r="D87" s="88"/>
-      <c r="E87" s="39">
-        <f>100-E86</f>
-        <v>9.3903340136651536</v>
-      </c>
-      <c r="F87" s="49"/>
-      <c r="G87" s="48"/>
-      <c r="H87" s="48"/>
-      <c r="I87" s="48"/>
-      <c r="J87" s="48"/>
-      <c r="K87" s="49"/>
-    </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A88" s="56"/>
-      <c r="B88" s="29" t="s">
+      <c r="C55" s="71">
+        <f>C52-C54</f>
+        <v>58164.145273680333</v>
+      </c>
+      <c r="D55" s="71"/>
+      <c r="E55" s="39">
+        <f>100-E54</f>
+        <v>9.4596742582527753</v>
+      </c>
+      <c r="F55" s="49"/>
+      <c r="G55" s="48"/>
+      <c r="H55" s="48"/>
+      <c r="I55" s="48"/>
+      <c r="J55" s="48"/>
+      <c r="K55" s="49"/>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A56" s="56"/>
+      <c r="B56" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C88" s="88">
-        <f>C85*0.03</f>
+      <c r="C56" s="71">
+        <f>C53*0.03</f>
         <v>17580</v>
       </c>
-      <c r="D88" s="88"/>
-      <c r="E88" s="39">
+      <c r="D56" s="71"/>
+      <c r="E56" s="39">
         <v>3</v>
       </c>
-      <c r="F88" s="49"/>
-      <c r="G88" s="48"/>
-      <c r="H88" s="48"/>
-      <c r="I88" s="48"/>
-      <c r="J88" s="48"/>
-      <c r="K88" s="49"/>
-    </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A89" s="56"/>
-      <c r="B89" s="29" t="s">
+      <c r="F56" s="49"/>
+      <c r="G56" s="48"/>
+      <c r="H56" s="48"/>
+      <c r="I56" s="48"/>
+      <c r="J56" s="48"/>
+      <c r="K56" s="49"/>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A57" s="56"/>
+      <c r="B57" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C89" s="88">
-        <f>C85*0.02</f>
+      <c r="C57" s="71">
+        <f>C53*0.02</f>
         <v>11720</v>
       </c>
-      <c r="D89" s="88"/>
-      <c r="E89" s="39">
+      <c r="D57" s="71"/>
+      <c r="E57" s="39">
         <v>2</v>
       </c>
-      <c r="F89" s="49"/>
-      <c r="G89" s="48"/>
-      <c r="H89" s="48"/>
-      <c r="I89" s="48"/>
-      <c r="J89" s="48"/>
-      <c r="K89" s="49"/>
-    </row>
-    <row r="90" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="57"/>
-      <c r="B90" s="57"/>
-      <c r="C90" s="57"/>
-      <c r="D90" s="57"/>
-      <c r="E90" s="57"/>
-      <c r="F90" s="57"/>
-      <c r="G90" s="57"/>
-      <c r="H90" s="57"/>
-      <c r="I90" s="57"/>
-      <c r="J90" s="57"/>
-      <c r="K90" s="57"/>
-    </row>
-    <row r="91" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="92" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="93" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="94" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="95" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="96" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+      <c r="F57" s="49"/>
+      <c r="G57" s="48"/>
+      <c r="H57" s="48"/>
+      <c r="I57" s="48"/>
+      <c r="J57" s="48"/>
+      <c r="K57" s="49"/>
+    </row>
+    <row r="58" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="57"/>
+      <c r="B58" s="57"/>
+      <c r="C58" s="57"/>
+      <c r="D58" s="57"/>
+      <c r="E58" s="57"/>
+      <c r="F58" s="57"/>
+      <c r="G58" s="57"/>
+      <c r="H58" s="57"/>
+      <c r="I58" s="57"/>
+      <c r="J58" s="57"/>
+      <c r="K58" s="57"/>
+    </row>
+    <row r="59" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="63" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="1:19" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="65" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="66" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="67" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="68" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="69" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="70" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="71" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="72" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="73" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="74" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="75" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="76" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="77" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="78" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="79" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="80" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="81" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="82" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="83" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="84" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="85" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="86" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="87" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="88" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="89" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="90" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="91" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="92" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="93" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="94" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="95" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="96" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="97" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="98" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="99" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -10779,55 +9979,23 @@
     <row r="112" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="113" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="114" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="115" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="116" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="117" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="118" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="119" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="120" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="121" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="122" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="123" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="124" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="125" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="126" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="127" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="128" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="129" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="130" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="131" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="132" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="133" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="134" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="135" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="136" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="137" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="138" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="139" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="140" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="141" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="142" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="143" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="144" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="145" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="146" s="35" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>

</xml_diff>